<commit_message>
Doc updated & Charts revised
</commit_message>
<xml_diff>
--- a/memory-graphs.xlsx
+++ b/memory-graphs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guido\Desktop\AA_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20F47E85-FB9E-4DF3-8EDD-1352E878AB77}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A66FC048-98F8-4B22-8DBB-857877118D14}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="6108" xr2:uid="{A47C4D61-F443-47CF-B379-EFF693CABE80}"/>
   </bookViews>
@@ -20,12 +20,17 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Tarjan</t>
   </si>
@@ -43,18 +48,6 @@
   </si>
   <si>
     <t>Normal</t>
-  </si>
-  <si>
-    <t>Sum</t>
-  </si>
-  <si>
-    <t>Average</t>
-  </si>
-  <si>
-    <t>Running Total</t>
-  </si>
-  <si>
-    <t>Count</t>
   </si>
 </sst>
 </file>
@@ -124,6 +117,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="150" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Profile memory usage</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -137,11 +155,11 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="150" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
@@ -175,13 +193,25 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
+            <a:pattFill prst="narHorz">
+              <a:fgClr>
+                <a:schemeClr val="accent1"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="20000"/>
+                  <a:lumOff val="80000"/>
+                </a:schemeClr>
+              </a:bgClr>
+            </a:pattFill>
             <a:ln>
               <a:noFill/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:innerShdw blurRad="114300">
+                <a:schemeClr val="accent1"/>
+              </a:innerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
@@ -208,13 +238,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>1204224</c:v>
+                  <c:v>1204.2239999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1552384</c:v>
+                  <c:v>1552.384</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1548288</c:v>
+                  <c:v>1548.288</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -240,13 +270,25 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
+            <a:pattFill prst="narHorz">
+              <a:fgClr>
+                <a:schemeClr val="accent2"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="20000"/>
+                  <a:lumOff val="80000"/>
+                </a:schemeClr>
+              </a:bgClr>
+            </a:pattFill>
             <a:ln>
               <a:noFill/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:innerShdw blurRad="114300">
+                <a:schemeClr val="accent2"/>
+              </a:innerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
@@ -273,13 +315,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>1122304</c:v>
+                  <c:v>1122.3040000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1486848</c:v>
+                  <c:v>1486.848</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1536000</c:v>
+                  <c:v>1536</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -305,13 +347,25 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent3"/>
-            </a:solidFill>
+            <a:pattFill prst="narHorz">
+              <a:fgClr>
+                <a:schemeClr val="accent3"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="20000"/>
+                  <a:lumOff val="80000"/>
+                </a:schemeClr>
+              </a:bgClr>
+            </a:pattFill>
             <a:ln>
               <a:noFill/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:innerShdw blurRad="114300">
+                <a:schemeClr val="accent3"/>
+              </a:innerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
@@ -338,13 +392,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>1105920</c:v>
+                  <c:v>1105.92</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1548288</c:v>
+                  <c:v>1548.288</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1540096</c:v>
+                  <c:v>1540.096</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -363,8 +417,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
+        <c:gapWidth val="164"/>
+        <c:overlap val="-22"/>
         <c:axId val="1116246112"/>
         <c:axId val="1176400192"/>
       </c:barChart>
@@ -375,17 +429,77 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Graph</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> category</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
               <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -426,20 +540,66 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Memory</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> KB</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
           <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-        </c:majorGridlines>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -484,7 +644,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="b"/>
+      <c:legendPos val="t"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -566,6 +726,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="150" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Profile memory usage</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -579,11 +764,11 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="150" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
@@ -617,13 +802,25 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
+            <a:pattFill prst="narHorz">
+              <a:fgClr>
+                <a:schemeClr val="accent1"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="20000"/>
+                  <a:lumOff val="80000"/>
+                </a:schemeClr>
+              </a:bgClr>
+            </a:pattFill>
             <a:ln>
               <a:noFill/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:innerShdw blurRad="114300">
+                <a:schemeClr val="accent1"/>
+              </a:innerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
@@ -650,13 +847,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>1204224</c:v>
+                  <c:v>1204.2239999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1122304</c:v>
+                  <c:v>1122.3040000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1105920</c:v>
+                  <c:v>1105.92</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -682,13 +879,25 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
+            <a:pattFill prst="narHorz">
+              <a:fgClr>
+                <a:schemeClr val="accent2"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="20000"/>
+                  <a:lumOff val="80000"/>
+                </a:schemeClr>
+              </a:bgClr>
+            </a:pattFill>
             <a:ln>
               <a:noFill/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:innerShdw blurRad="114300">
+                <a:schemeClr val="accent2"/>
+              </a:innerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
@@ -715,13 +924,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>1552384</c:v>
+                  <c:v>1552.384</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1486848</c:v>
+                  <c:v>1486.848</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1548288</c:v>
+                  <c:v>1548.288</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -747,13 +956,25 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent3"/>
-            </a:solidFill>
+            <a:pattFill prst="narHorz">
+              <a:fgClr>
+                <a:schemeClr val="accent3"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="20000"/>
+                  <a:lumOff val="80000"/>
+                </a:schemeClr>
+              </a:bgClr>
+            </a:pattFill>
             <a:ln>
               <a:noFill/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:innerShdw blurRad="114300">
+                <a:schemeClr val="accent3"/>
+              </a:innerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
@@ -780,13 +1001,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>1548288</c:v>
+                  <c:v>1548.288</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1536000</c:v>
+                  <c:v>1536</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1540096</c:v>
+                  <c:v>1540.096</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -805,8 +1026,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
+        <c:gapWidth val="164"/>
+        <c:overlap val="-22"/>
         <c:axId val="1116244112"/>
         <c:axId val="1112742912"/>
       </c:barChart>
@@ -817,17 +1038,72 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Algorithms</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
               <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -868,20 +1144,61 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Memory KB</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
           <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-        </c:majorGridlines>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -926,7 +1243,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="b"/>
+      <c:legendPos val="t"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1074,7 +1391,7 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="203">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -1085,7 +1402,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
@@ -1098,11 +1415,11 @@
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1115,7 +1432,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -1131,7 +1448,7 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
@@ -1175,32 +1492,70 @@
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="narHorz">
+        <a:fgClr>
+          <a:schemeClr val="phClr"/>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:bgClr>
+      </a:pattFill>
+      <a:effectLst>
+        <a:innerShdw blurRad="114300">
+          <a:schemeClr val="phClr"/>
+        </a:innerShdw>
+      </a:effectLst>
+    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="narHorz">
+        <a:fgClr>
+          <a:schemeClr val="phClr"/>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:bgClr>
+      </a:pattFill>
+      <a:effectLst>
+        <a:innerShdw blurRad="114300">
+          <a:schemeClr val="phClr"/>
+        </a:innerShdw>
+      </a:effectLst>
+    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="28575" cap="rnd">
@@ -1212,33 +1567,29 @@
     </cs:spPr>
   </cs:dataPointLine>
   <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -1260,15 +1611,13 @@
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -1283,15 +1632,15 @@
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -1302,10 +1651,10 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
@@ -1321,14 +1670,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1340,31 +1689,24 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
   </cs:floor>
   <cs:gridlineMajor>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:gridlineMajor>
@@ -1373,17 +1715,16 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="5000"/>
             <a:lumOff val="95000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:gridlineMinor>
@@ -1392,29 +1733,10 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
@@ -1422,6 +1744,24 @@
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
       </a:ln>
     </cs:spPr>
   </cs:leaderLine>
@@ -1442,7 +1782,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
   </cs:plotArea>
   <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
@@ -1450,7 +1790,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
   </cs:plotArea3D>
   <cs:seriesAxis>
@@ -1470,10 +1810,10 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
@@ -1490,11 +1830,11 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+    <cs:defRPr sz="1800" b="1" kern="1200" cap="all" spc="150" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -1503,14 +1843,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:prstDash val="sysDot"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -1540,8 +1879,8 @@
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -1564,20 +1903,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="203">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -1588,7 +1921,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
@@ -1601,11 +1934,11 @@
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1618,7 +1951,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -1634,7 +1967,7 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
@@ -1678,32 +2011,70 @@
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="narHorz">
+        <a:fgClr>
+          <a:schemeClr val="phClr"/>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:bgClr>
+      </a:pattFill>
+      <a:effectLst>
+        <a:innerShdw blurRad="114300">
+          <a:schemeClr val="phClr"/>
+        </a:innerShdw>
+      </a:effectLst>
+    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="narHorz">
+        <a:fgClr>
+          <a:schemeClr val="phClr"/>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:bgClr>
+      </a:pattFill>
+      <a:effectLst>
+        <a:innerShdw blurRad="114300">
+          <a:schemeClr val="phClr"/>
+        </a:innerShdw>
+      </a:effectLst>
+    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="28575" cap="rnd">
@@ -1715,33 +2086,29 @@
     </cs:spPr>
   </cs:dataPointLine>
   <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -1763,15 +2130,13 @@
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -1786,15 +2151,15 @@
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -1805,10 +2170,10 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
@@ -1824,14 +2189,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1843,31 +2208,24 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
   </cs:floor>
   <cs:gridlineMajor>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:gridlineMajor>
@@ -1876,17 +2234,16 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="5000"/>
             <a:lumOff val="95000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:gridlineMinor>
@@ -1895,29 +2252,10 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
@@ -1925,6 +2263,24 @@
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
       </a:ln>
     </cs:spPr>
   </cs:leaderLine>
@@ -1945,7 +2301,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
   </cs:plotArea>
   <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
@@ -1953,7 +2309,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
   </cs:plotArea3D>
   <cs:seriesAxis>
@@ -1973,10 +2329,10 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
@@ -1993,11 +2349,11 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+    <cs:defRPr sz="1800" b="1" kern="1200" cap="all" spc="150" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -2006,14 +2362,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:prstDash val="sysDot"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -2043,8 +2398,8 @@
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -2067,14 +2422,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -2456,7 +2805,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E4"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2477,13 +2826,16 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>1204224</v>
+        <f>1204224/1000</f>
+        <v>1204.2239999999999</v>
       </c>
       <c r="C2">
-        <v>1122304</v>
+        <f>1122304/1000</f>
+        <v>1122.3040000000001</v>
       </c>
       <c r="D2">
-        <v>1105920</v>
+        <f>1105920/1000</f>
+        <v>1105.92</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -2491,13 +2843,16 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>1552384</v>
+        <f>1552384/1000</f>
+        <v>1552.384</v>
       </c>
       <c r="C3">
-        <v>1486848</v>
+        <f>1486848/1000</f>
+        <v>1486.848</v>
       </c>
       <c r="D3">
-        <v>1548288</v>
+        <f>1548288/1000</f>
+        <v>1548.288</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -2505,13 +2860,16 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>1548288</v>
+        <f>1548288/1000</f>
+        <v>1548.288</v>
       </c>
       <c r="C4">
-        <v>1536000</v>
+        <f>1536000/1000</f>
+        <v>1536</v>
       </c>
       <c r="D4">
-        <v>1540096</v>
+        <f>1540096/1000</f>
+        <v>1540.096</v>
       </c>
     </row>
   </sheetData>

</xml_diff>